<commit_message>
new parameters added ; deleted old masterfile
</commit_message>
<xml_diff>
--- a/resources/lang/MasterFile FightNight.xlsx
+++ b/resources/lang/MasterFile FightNight.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="210">
   <si>
     <t>Keys</t>
   </si>
@@ -693,15 +693,303 @@
                 &lt;/ul&gt;
                 &lt;p&gt;We also agree to the Individual Redress Principle which requires that individuals have the right to legally pursue enforceable rights against data collectors and processors who fail to adhere to the law. This principle requires not only that individuals have enforceable rights against data users, but also that individuals have recourse to courts or government agencies to investigate and/or prosecute non-compliance by data processors.&lt;/p&gt;</t>
   </si>
+  <si>
+    <t>// Contact</t>
+  </si>
+  <si>
+    <t>contact_title</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>&lt;span class="city"&gt;Saint-Tropez&lt;/span&gt; Fight Night &lt;span class="year"&gt;2017&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Résultats</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>results</t>
+  </si>
+  <si>
+    <t>editions_title</t>
+  </si>
+  <si>
+    <t>// Editions</t>
+  </si>
+  <si>
+    <t>all_albums</t>
+  </si>
+  <si>
+    <t>All albums</t>
+  </si>
+  <si>
+    <t>Tous les albums</t>
+  </si>
+  <si>
+    <t>title_year</t>
+  </si>
+  <si>
+    <t>Title / year</t>
+  </si>
+  <si>
+    <t>// Index</t>
+  </si>
+  <si>
+    <t>discover</t>
+  </si>
+  <si>
+    <t>Discover</t>
+  </si>
+  <si>
+    <t>// Presse</t>
+  </si>
+  <si>
+    <t>presse</t>
+  </si>
+  <si>
+    <t>in_presse</t>
+  </si>
+  <si>
+    <t>In the press</t>
+  </si>
+  <si>
+    <t>La presse en parle</t>
+  </si>
+  <si>
+    <t>site mail</t>
+  </si>
+  <si>
+    <t>info@fightnights.pro</t>
+  </si>
+  <si>
+    <t>// Mail</t>
+  </si>
+  <si>
+    <t>// Results Content</t>
+  </si>
+  <si>
+    <t>results_content_1</t>
+  </si>
+  <si>
+    <t>&lt;h1 class="title--translated"&gt;Résultats 2013&lt;/h1&gt;
+                    &lt;h3&gt;CHAMPIONNAT DU MONDE WKN&lt;/h3&gt;
+                    &lt;p&gt;Kick boxing . 5×2 mn . +100kg&lt;br&gt;
+                        Vainqueur : Jerome LE BANNER par KO2
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        Kick boxing . 5×2 mn . -100kg&lt;br&gt;
+                        Vainqueur : Wladimir MINEEV aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        Kick boxing . 5×2 mn . -96,600kg&lt;br&gt;
+                        Vainqueur : Emmanuel PAYET aux points
+                    &lt;/p&gt;
+                    &lt;h3&gt;MASTERFIGHT&lt;/h3&gt;
+                    &lt;p&gt;
+                        PRO FIGHT . 3×2 mn (1Extra Round) . + 95kg&lt;br&gt;
+                        Vainqueur : Anthony REA par KO1
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        PRO FIGHT . 3×2 mn (1Extra Round) . -70kg&lt;br&gt;
+                        Vainqueur : Philippe SALMON KO1
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        PRO FIGHT . 3×2 mn (1Extra Round) . -95kg&lt;br&gt;
+                        Vainqueur : Zinedine Hameur Lain aux points
+                    &lt;/p&gt;
+                    &lt;h3&gt;SUPERFIGHT&lt;/h3&gt;
+                    &lt;p&gt;
+                        K-1 . 4×2 mn . +100kg&lt;br&gt;
+                        Vainqueur : Nicolas WAMBA par KO4
+                    &lt;/p&gt;
+                    &lt;h3&gt;SUPERFIGHT (FÉMININ)&lt;/h3&gt;
+                    &lt;p&gt;
+                        K-1 . 4×2 mn . -58,500kg&lt;br&gt;
+                        Vainqueur : Alena Ola aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        K-1 . 4×2 mn . +100kg&lt;br&gt;
+                        Vainqueur : Luca PANTO aux points
+                    &lt;/p&gt;
+                    &lt;h3&gt;TOURNOI MASTERFIGHT&lt;/h3&gt;
+                    &lt;p&gt;
+                        Finale PRO FIGHT . 3×2 mn (1Extra Round) . -82kg&lt;br&gt;
+                        Vainqueur : Yoan KONGOLO par KO2
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        Demi finale PRO FIGHT . 3×2 mn (1Extra Round) . -82kg&lt;br&gt;
+                        Vainqueur : Yoan KONGOLO aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        Demi finale PRO FIGHT . 3×2 mn (1Extra Round) . -82kg&lt;br&gt;
+                        Vainqueur : Francky BRUCTER aux points
+                    &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>results_content_2</t>
+  </si>
+  <si>
+    <t>&lt;h1 class="title--translated"&gt;Résultats 2014&lt;/h1&gt;
+                    &lt;p&gt;
+                        + 110.600 KG&lt;br&gt;
+                        Victoire Jérôme Le Banner (Fra) par KO2
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        + 110.600 KG&lt;br&gt;
+                        Victoire Freddy Kemayo (Fra) arr arbitre 2e
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        -96.400 KG&lt;br&gt;
+                        Victoire Vladimir Mineev (Russie) aux Points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        -110.600 KG&lt;br&gt;
+                        Victoire Nicolas Wamba (Fra) par KO2
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        -63.500 KG&lt;br&gt;
+                        Victoire Maneenoi Ekkarit (Tha) par KO1
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        -96.400 KG&lt;br&gt;
+                        Victoire Filip Verlinden (Bel) aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        -66.100 KG&lt;br&gt;
+                        Victoire Samsamut Kietchongkao (Tha) aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        -80.500 KG&lt;br&gt;
+                        Victoire Yohann Kongolo (Sui) aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        -58.200 KG&lt;br&gt;
+                        Victoire Taehiran Chommanee (Tha) aux points
+                    &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>Retour aux editions</t>
+  </si>
+  <si>
+    <t>Back to the editions</t>
+  </si>
+  <si>
+    <t>results_content_3</t>
+  </si>
+  <si>
+    <t>&lt;h1 class="title--translated"&gt;Résultats 2015&lt;/h1&gt;
+                    &lt;h3&gt;KICK-BOXING&lt;/h3&gt;
+                    &lt;p&gt;
+                        75KG&lt;br&gt;
+                        Sharos Huyer bat Bakari Tounkara aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        100KG&lt;br&gt;
+                        Frank Munoz bat Zinedine Hameur Lain  aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        120KG&lt;br&gt;
+                        Fabrice Aurieng bat Yuksel Ayadi aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        95KG&lt;br&gt;
+                        Alexey Papin bat Danyo Ilunga aux points
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        93KG&lt;br&gt;
+                        Alexander Vezhevatov bat Filip Verlinden aux points
+                    &lt;/p&gt;
+                    &lt;h3&gt;CHAMPIONNAT DU MONDE  – WKN&lt;/h3&gt;
+                    &lt;p&gt;
+                        120 KG&lt;br&gt;
+                        Jerome LEBANNER bat Karl ROBERSON aux points
+                    &lt;/p&gt;
+                    &lt;h3&gt;MUAYTHAI&lt;/h3&gt;
+                    &lt;p&gt;
+                        71 KG&lt;br&gt;
+                        Yodwicha Por Boonsit (THA) bat aux pts Jimmy Viennot (F)
+                    &lt;/p&gt;
+                    &lt;p&gt;
+                        77 KG&lt;br&gt;
+                        Yohan LIDON bat Jonathan OLIVEIRA par TKO3
+                    &lt;/p&gt;
+                    &lt;h3&gt;CHAMPIONNAT DU MONDE  – WMC EN 52KG&lt;/h3&gt;
+                    &lt;p&gt;Lizzie LARGILLIERE bat Petchoydying MOR par abandon à l’appel de R5&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>results_content_4</t>
+  </si>
+  <si>
+    <t>&lt;h1 class="title--translated"&gt;Résultats 2016&lt;/h1&gt;
+                    &lt;h3&gt;SUPERFIGHT . MUAYTHAI . 3×3 MN . -67KG&lt;/h3&gt;
+                    &lt;p&gt;
+                        Vainqueur : Dylan Salvador par TKO2
+                    &lt;/p&gt;
+                    &lt;h3&gt;500KG TOURNAMENT . DEMI FINALE . 3×3 MN . K-1 RULES . +110KG&lt;/h3&gt;
+                    &lt;p&gt;
+                        Vainqueur : Thomas Vanneste aux points
+                    &lt;/p&gt;
+                    &lt;h3&gt;500KG TOURNAMENT . DEMI FINALE . 3×3 MN . K-1 RULES . +110KG&lt;/h3&gt;
+                    &lt;p&gt;
+                        Vainqueur : Tomas Mozny aux points
+                    &lt;/p&gt;
+                    &lt;h3&gt;SUPERFIGHT . K-1 RULES . 3×3 MN . -96KG&lt;/h3&gt;
+                    &lt;p&gt;
+                        Vainqueur : Mikhael Tiuterev aux points
+                    &lt;/p&gt;
+                    &lt;h3&gt;CHAMPIONNAT DU MONDE WMC . MUAYTHAI . 5×3 MN . -57,200KG&lt;/h3&gt;
+                    &lt;p&gt;Vainqueur : Taiheran Chomanee aux points&lt;/p&gt;
+                    &lt;h3&gt;SUPERFIGHT . K-1 RULES . 3×3 MN . -96KG&lt;/h3&gt;
+                    &lt;p&gt;Vainqueur : Stéphane Susperregui aux points&lt;/p&gt;
+                    &lt;h3&gt;500KG TOURNAMENT . DEMI FINALE . 3×3 MN . K-1 RULES . +110KG&lt;/h3&gt;
+                    &lt;p&gt;Vainqueur : Tomas Mozny aux points&lt;/p&gt;
+                    &lt;h3&gt;CHAMPIONNAT DU MONDE WKN . K-1 RULES . 5×3 MN . -76,600KG&lt;/h3&gt;
+                    &lt;p&gt;Vainqueur : Yohan Lidon aux points&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>results_content_5</t>
+  </si>
+  <si>
+    <t>&lt;h1 class="title--translated"&gt;Résultats 2017&lt;/h1&gt;
+                    &lt;h3&gt;CHAMPIONNAT DU MONDE WKN . K-1  (79,4 KG)&lt;/h3&gt;
+                    &lt;p&gt;Yohan LIDON bat Florian KROGER par KO au round 4 (highkick)&lt;/p&gt;
+                    &lt;h3&gt;SUPERFIGHT . MUAYTHAI&lt;/h3&gt;
+                    &lt;p&gt;Umar SEMATA bat Evgeny KURAVSKOI par décision&lt;/p&gt;
+                    &lt;h3&gt;SUPERFIGHT . K-1&lt;/h3&gt;
+                    &lt;p&gt;Grégory TONY bat Bob SAPP par KO au round 1&lt;/p&gt;
+                    &lt;p&gt;Mikhail CHALYKH  bat Phillip VERLINDEN par décision&lt;/p&gt;
+                    &lt;p&gt;Stéphane SUSPERREGUI bat Danyo ILUNGA par décision (unanime)&lt;/p&gt;
+                    &lt;p&gt;Tomas MOZNY bat Daniel SAM par décision&lt;/p&gt;
+                    &lt;p&gt;Tomas MOZNY bat Daniel SAM par décision&lt;/p&gt;
+                    &lt;p&gt;Mallaury KALASHNIKOFF bat Marina SPASIC par décision (unanime)&lt;/p&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -736,10 +1024,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -751,8 +1040,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1031,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:C75"/>
+  <dimension ref="A6:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,8 +2069,199 @@
         <v>169</v>
       </c>
     </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>170</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>172</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>178</v>
+      </c>
+      <c r="B82" t="s">
+        <v>174</v>
+      </c>
+      <c r="C82" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>177</v>
+      </c>
+      <c r="B83" t="s">
+        <v>175</v>
+      </c>
+      <c r="C83" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" t="s">
+        <v>184</v>
+      </c>
+      <c r="C86" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>186</v>
+      </c>
+      <c r="B87" t="s">
+        <v>187</v>
+      </c>
+      <c r="C87" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>189</v>
+      </c>
+      <c r="B90" t="s">
+        <v>59</v>
+      </c>
+      <c r="C90" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>190</v>
+      </c>
+      <c r="B91" t="s">
+        <v>192</v>
+      </c>
+      <c r="C91" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>193</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>197</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>199</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>201</v>
+      </c>
+      <c r="B98" t="s">
+        <v>202</v>
+      </c>
+      <c r="C98" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>204</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>206</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>208</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B93" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>